<commit_message>
Fixed problem where a fixed asset value was overridden if an amount was added each year after that
</commit_message>
<xml_diff>
--- a/tests/Feature/config/fond_zero.xlsx
+++ b/tests/Feature/config/fond_zero.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="private" sheetId="1" r:id="rId4"/>
-    <sheet name="Salary" sheetId="2" r:id="rId5"/>
+    <sheet name="Income" sheetId="2" r:id="rId5"/>
     <sheet name="fond privat" sheetId="3" r:id="rId6"/>
     <sheet name="Statistics" sheetId="4" r:id="rId7"/>
   </sheets>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>private</t>
   </si>
@@ -137,28 +137,25 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Salary</t>
+    <t>Income</t>
   </si>
   <si>
-    <t>salary</t>
+    <t>income</t>
   </si>
   <si>
     <t xml:space="preserve">Using previous value: 0Using previous value: 0 Asset rule </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule </t>
+    <t xml:space="preserve">Using previous value: 0 Asset rule </t>
   </si>
   <si>
-    <t xml:space="preserve">SalaryNormal: 480000Normal: 180000 Asset rule </t>
+    <t xml:space="preserve">IncomeNormal: 480000Normal: 180000 Asset rule </t>
   </si>
   <si>
-    <t xml:space="preserve">Using previous value: 480000Using previous value: 180000 Asset rule </t>
+    <t xml:space="preserve">Using previous value: 0Using previous value: 180000 Asset rule </t>
   </si>
   <si>
     <t xml:space="preserve">Pensioned, no more salary from hereFixed number override = detected: 0Using previous value: 180000 Asset rule </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using previous value: 180000 Asset rule </t>
   </si>
   <si>
     <t>fond privat</t>
@@ -167,86 +164,86 @@
     <t>fond</t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule Normal: 100000</t>
+    <t>Using previous value: 0 Asset rule Normal: 100000</t>
   </si>
   <si>
-    <t xml:space="preserve">Uttak fra 2037, -1/20 Asset rule -1/19Adding divisor rule: -1/19 transfer diff 5 000,00 to salary.2037.income.amount
+    <t xml:space="preserve">Using previous value: 0Uttak fra 2037, -1/20 Asset rule -1/19Adding divisor rule: -1/19 transfer diff 5 000,00 to income.2037.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/18Adding previous divisor rule: -1/18 transfer diff 5 000,00 to salary.2038.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/18Error rule: -1/18 transfer diff 5 000,00 to income.2038.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/17Adding previous divisor rule: -1/17 transfer diff 5 000,00 to salary.2039.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/17Error rule: -1/17 transfer diff 5 000,00 to income.2039.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/16Adding previous divisor rule: -1/16 transfer diff 5 000,00 to salary.2040.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/16Error rule: -1/16 transfer diff 5 000,00 to income.2040.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/15Adding previous divisor rule: -1/15 transfer diff 5 000,00 to salary.2041.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/15Error rule: -1/15 transfer diff 5 000,00 to income.2041.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/14Adding previous divisor rule: -1/14 transfer diff 5 000,00 to salary.2042.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/14Error rule: -1/14 transfer diff 5 000,00 to income.2042.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/13Adding previous divisor rule: -1/13 transfer diff 5 000,00 to salary.2043.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/13Error rule: -1/13 transfer diff 5 000,00 to income.2043.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/12Adding previous divisor rule: -1/12 transfer diff 5 000,00 to salary.2044.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/12Error rule: -1/12 transfer diff 5 000,00 to income.2044.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/11Adding previous divisor rule: -1/11 transfer diff 5 000,00 to salary.2045.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/11Error rule: -1/11 transfer diff 5 000,00 to income.2045.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/10Adding previous divisor rule: -1/10 transfer diff 5 000,00 to salary.2046.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/10Error rule: -1/10 transfer diff 5 000,00 to income.2046.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/9Adding previous divisor rule: -1/9 transfer diff 5 000,00 to salary.2047.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/9Error rule: -1/9 transfer diff 5 000,00 to income.2047.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/8Adding previous divisor rule: -1/8 transfer diff 5 000,00 to salary.2048.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/8Error rule: -1/8 transfer diff 5 000,00 to income.2048.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/7Adding previous divisor rule: -1/7 transfer diff 5 000,00 to salary.2049.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/7Error rule: -1/7 transfer diff 5 000,00 to income.2049.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/6Adding previous divisor rule: -1/6 transfer diff 5 000,00 to salary.2050.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/6Error rule: -1/6 transfer diff 5 000,00 to income.2050.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/5Adding previous divisor rule: -1/5 transfer diff 5 000,00 to salary.2051.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/5Error rule: -1/5 transfer diff 5 000,00 to income.2051.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/4Adding previous divisor rule: -1/4 transfer diff 5 000,00 to salary.2052.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/4Error rule: -1/4 transfer diff 5 000,00 to income.2052.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/3Adding previous divisor rule: -1/3 transfer diff 5 000,00 to salary.2053.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/3Error rule: -1/3 transfer diff 5 000,00 to income.2053.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/2Adding previous divisor rule: -1/2 transfer diff 5 000,00 to salary.2054.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/2Error rule: -1/2 transfer diff 5 000,00 to income.2054.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule -1/1Adding previous divisor rule: -1/1 transfer diff 5 000,00 to salary.2055.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule -1/1Error rule: -1/1 transfer diff 5 000,00 to income.2055.income.amount
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule Adding previous divisor rule:  transfer diff 5 000,00 to salary.2056.income.amount
+    <t xml:space="preserve">Using previous value: 0 Asset rule Error rule:  transfer diff 5 000,00 to income.2056.income.amount
 </t>
   </si>
   <si>
@@ -665,7 +662,7 @@
     <col min="10" max="10" width="37.705" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="9.283" bestFit="true" customWidth="true" style="0"/>
@@ -3155,7 +3152,7 @@
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="1">
@@ -3173,7 +3170,7 @@
         <v>0.0</v>
       </c>
       <c r="U38" s="6">
-        <v>60000.0</v>
+        <v>300000.0</v>
       </c>
       <c r="V38" s="1">
         <v>0.0</v>
@@ -3192,10 +3189,10 @@
         <v>0.0</v>
       </c>
       <c r="AB38">
-        <v>60000.0</v>
+        <v>300000.0</v>
       </c>
       <c r="AC38" s="2">
-        <v>0.125</v>
+        <v>0.625</v>
       </c>
       <c r="AD38"/>
     </row>
@@ -3207,7 +3204,7 @@
         <v>49</v>
       </c>
       <c r="C39" s="8">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="8">
@@ -3229,7 +3226,7 @@
       </c>
       <c r="L39" s="9"/>
       <c r="M39" s="8">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N39" s="9"/>
       <c r="O39" s="8">
@@ -3249,29 +3246,29 @@
         <v>0.0</v>
       </c>
       <c r="U39" s="8">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V39" s="8">
         <v>100000.0</v>
       </c>
       <c r="W39" s="9"/>
       <c r="X39" s="8">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y39" s="8">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z39" s="8">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA39" s="7">
         <v>0.0</v>
       </c>
       <c r="AB39" s="7">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC39" s="9">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD39" s="7"/>
     </row>
@@ -3283,7 +3280,7 @@
         <v>50</v>
       </c>
       <c r="C40" s="11">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="11">
@@ -3305,7 +3302,7 @@
       </c>
       <c r="L40" s="12"/>
       <c r="M40" s="11">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N40" s="12"/>
       <c r="O40" s="11">
@@ -3325,29 +3322,29 @@
         <v>0.0</v>
       </c>
       <c r="U40" s="11">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V40" s="11">
         <v>100000.0</v>
       </c>
       <c r="W40" s="12"/>
       <c r="X40" s="11">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y40" s="11">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z40" s="11">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA40" s="10">
         <v>0.0</v>
       </c>
       <c r="AB40" s="10">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC40" s="12">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD40" s="10"/>
     </row>
@@ -3359,7 +3356,7 @@
         <v>51</v>
       </c>
       <c r="C41" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="5">
@@ -3381,7 +3378,7 @@
       </c>
       <c r="L41" s="2"/>
       <c r="M41" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="1">
@@ -3401,29 +3398,29 @@
         <v>0.0</v>
       </c>
       <c r="U41" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V41" s="1">
         <v>100000.0</v>
       </c>
       <c r="W41" s="2"/>
       <c r="X41" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y41" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z41" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA41">
         <v>0.0</v>
       </c>
       <c r="AB41">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC41" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD41"/>
     </row>
@@ -3435,7 +3432,7 @@
         <v>52</v>
       </c>
       <c r="C42" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="5">
@@ -3457,7 +3454,7 @@
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="1">
@@ -3477,29 +3474,29 @@
         <v>0.0</v>
       </c>
       <c r="U42" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V42" s="1">
         <v>100000.0</v>
       </c>
       <c r="W42" s="2"/>
       <c r="X42" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y42" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z42" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA42">
         <v>0.0</v>
       </c>
       <c r="AB42">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC42" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD42"/>
     </row>
@@ -3511,7 +3508,7 @@
         <v>53</v>
       </c>
       <c r="C43" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="5">
@@ -3533,7 +3530,7 @@
       </c>
       <c r="L43" s="2"/>
       <c r="M43" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="1">
@@ -3553,29 +3550,29 @@
         <v>0.0</v>
       </c>
       <c r="U43" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V43" s="1">
         <v>100000.0</v>
       </c>
       <c r="W43" s="2"/>
       <c r="X43" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y43" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z43" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA43">
         <v>0.0</v>
       </c>
       <c r="AB43">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC43" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD43"/>
     </row>
@@ -3587,7 +3584,7 @@
         <v>54</v>
       </c>
       <c r="C44" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="5">
@@ -3609,7 +3606,7 @@
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="1">
@@ -3629,29 +3626,29 @@
         <v>0.0</v>
       </c>
       <c r="U44" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V44" s="1">
         <v>100000.0</v>
       </c>
       <c r="W44" s="2"/>
       <c r="X44" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y44" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z44" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA44">
         <v>0.0</v>
       </c>
       <c r="AB44">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC44" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD44"/>
     </row>
@@ -3663,7 +3660,7 @@
         <v>55</v>
       </c>
       <c r="C45" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5">
@@ -3685,7 +3682,7 @@
       </c>
       <c r="L45" s="2"/>
       <c r="M45" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="1">
@@ -3705,29 +3702,29 @@
         <v>0.0</v>
       </c>
       <c r="U45" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V45" s="1">
         <v>100000.0</v>
       </c>
       <c r="W45" s="2"/>
       <c r="X45" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y45" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z45" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA45">
         <v>0.0</v>
       </c>
       <c r="AB45">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC45" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD45"/>
     </row>
@@ -3739,7 +3736,7 @@
         <v>56</v>
       </c>
       <c r="C46" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="5">
@@ -3761,7 +3758,7 @@
       </c>
       <c r="L46" s="2"/>
       <c r="M46" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="1">
@@ -3781,29 +3778,29 @@
         <v>0.0</v>
       </c>
       <c r="U46" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V46" s="1">
         <v>100000.0</v>
       </c>
       <c r="W46" s="2"/>
       <c r="X46" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y46" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z46" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA46">
         <v>0.0</v>
       </c>
       <c r="AB46">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC46" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD46"/>
     </row>
@@ -3815,7 +3812,7 @@
         <v>57</v>
       </c>
       <c r="C47" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5">
@@ -3837,7 +3834,7 @@
       </c>
       <c r="L47" s="2"/>
       <c r="M47" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="1">
@@ -3857,29 +3854,29 @@
         <v>0.0</v>
       </c>
       <c r="U47" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V47" s="1">
         <v>100000.0</v>
       </c>
       <c r="W47" s="2"/>
       <c r="X47" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y47" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z47" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA47">
         <v>0.0</v>
       </c>
       <c r="AB47">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC47" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD47"/>
     </row>
@@ -3891,7 +3888,7 @@
         <v>58</v>
       </c>
       <c r="C48" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="5">
@@ -3913,7 +3910,7 @@
       </c>
       <c r="L48" s="2"/>
       <c r="M48" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="1">
@@ -3933,29 +3930,29 @@
         <v>0.0</v>
       </c>
       <c r="U48" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V48" s="1">
         <v>100000.0</v>
       </c>
       <c r="W48" s="2"/>
       <c r="X48" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y48" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z48" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA48">
         <v>0.0</v>
       </c>
       <c r="AB48">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC48" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD48"/>
     </row>
@@ -3967,7 +3964,7 @@
         <v>59</v>
       </c>
       <c r="C49" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="5">
@@ -3989,7 +3986,7 @@
       </c>
       <c r="L49" s="2"/>
       <c r="M49" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="1">
@@ -4009,29 +4006,29 @@
         <v>0.0</v>
       </c>
       <c r="U49" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V49" s="1">
         <v>100000.0</v>
       </c>
       <c r="W49" s="2"/>
       <c r="X49" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y49" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z49" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA49">
         <v>0.0</v>
       </c>
       <c r="AB49">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC49" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD49"/>
     </row>
@@ -4043,7 +4040,7 @@
         <v>60</v>
       </c>
       <c r="C50" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="5">
@@ -4065,7 +4062,7 @@
       </c>
       <c r="L50" s="2"/>
       <c r="M50" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="1">
@@ -4085,29 +4082,29 @@
         <v>0.0</v>
       </c>
       <c r="U50" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V50" s="1">
         <v>100000.0</v>
       </c>
       <c r="W50" s="2"/>
       <c r="X50" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y50" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z50" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA50">
         <v>0.0</v>
       </c>
       <c r="AB50">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC50" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD50"/>
     </row>
@@ -4119,7 +4116,7 @@
         <v>61</v>
       </c>
       <c r="C51" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="5">
@@ -4141,7 +4138,7 @@
       </c>
       <c r="L51" s="2"/>
       <c r="M51" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="1">
@@ -4161,29 +4158,29 @@
         <v>0.0</v>
       </c>
       <c r="U51" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V51" s="1">
         <v>100000.0</v>
       </c>
       <c r="W51" s="2"/>
       <c r="X51" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y51" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z51" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA51">
         <v>0.0</v>
       </c>
       <c r="AB51">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC51" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD51"/>
     </row>
@@ -4195,7 +4192,7 @@
         <v>62</v>
       </c>
       <c r="C52" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="5">
@@ -4217,7 +4214,7 @@
       </c>
       <c r="L52" s="2"/>
       <c r="M52" s="1">
-        <v>-240000.0</v>
+        <v>0.0</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="1">
@@ -4237,29 +4234,29 @@
         <v>0.0</v>
       </c>
       <c r="U52" s="6">
-        <v>59200.0</v>
+        <v>-180800.0</v>
       </c>
       <c r="V52" s="1">
         <v>100000.0</v>
       </c>
       <c r="W52" s="2"/>
       <c r="X52" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y52" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z52" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="AA52">
         <v>0.0</v>
       </c>
       <c r="AB52">
-        <v>64000.0</v>
+        <v>-176000.0</v>
       </c>
       <c r="AC52" s="2">
-        <v>0.13223140495868</v>
+        <v>-44.0</v>
       </c>
       <c r="AD52"/>
     </row>
@@ -6044,7 +6041,7 @@
     <col min="10" max="10" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="8.141" bestFit="true" customWidth="true" style="0"/>
@@ -6224,15 +6221,11 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L6" s="2"/>
       <c r="M6" s="1">
         <v>0.0</v>
       </c>
-      <c r="N6" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N6" s="2"/>
       <c r="O6" s="1">
         <v>0</v>
       </c>
@@ -6241,7 +6234,7 @@
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="1">
@@ -6292,15 +6285,11 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L7" s="2"/>
       <c r="M7" s="1">
         <v>0.0</v>
       </c>
-      <c r="N7" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N7" s="2"/>
       <c r="O7" s="1">
         <v>0</v>
       </c>
@@ -6309,7 +6298,7 @@
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="1">
@@ -6360,15 +6349,11 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L8" s="2"/>
       <c r="M8" s="1">
         <v>0.0</v>
       </c>
-      <c r="N8" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N8" s="2"/>
       <c r="O8" s="1">
         <v>0</v>
       </c>
@@ -6377,7 +6362,7 @@
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="1">
@@ -6428,15 +6413,11 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L9" s="2"/>
       <c r="M9" s="1">
         <v>0.0</v>
       </c>
-      <c r="N9" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N9" s="2"/>
       <c r="O9" s="1">
         <v>0</v>
       </c>
@@ -6445,7 +6426,7 @@
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="1">
@@ -6496,15 +6477,11 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L10" s="2"/>
       <c r="M10" s="1">
         <v>0.0</v>
       </c>
-      <c r="N10" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N10" s="2"/>
       <c r="O10" s="1">
         <v>0</v>
       </c>
@@ -6513,7 +6490,7 @@
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="1">
@@ -6564,15 +6541,11 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L11" s="2"/>
       <c r="M11" s="1">
         <v>0.0</v>
       </c>
-      <c r="N11" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N11" s="2"/>
       <c r="O11" s="1">
         <v>0</v>
       </c>
@@ -6581,7 +6554,7 @@
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="1">
@@ -6632,15 +6605,11 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L12" s="2"/>
       <c r="M12" s="1">
         <v>0.0</v>
       </c>
-      <c r="N12" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N12" s="2"/>
       <c r="O12" s="1">
         <v>0</v>
       </c>
@@ -6649,7 +6618,7 @@
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="1">
@@ -6700,15 +6669,11 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L13" s="2"/>
       <c r="M13" s="1">
         <v>0.0</v>
       </c>
-      <c r="N13" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N13" s="2"/>
       <c r="O13" s="1">
         <v>0</v>
       </c>
@@ -6717,7 +6682,7 @@
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="1">
@@ -6768,15 +6733,11 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L14" s="2"/>
       <c r="M14" s="1">
         <v>0.0</v>
       </c>
-      <c r="N14" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N14" s="2"/>
       <c r="O14" s="1">
         <v>0</v>
       </c>
@@ -6785,7 +6746,7 @@
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="1">
@@ -6836,15 +6797,11 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L15" s="2"/>
       <c r="M15" s="1">
         <v>0.0</v>
       </c>
-      <c r="N15" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N15" s="2"/>
       <c r="O15" s="1">
         <v>0</v>
       </c>
@@ -6853,7 +6810,7 @@
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="1">
@@ -6904,15 +6861,11 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L16" s="2"/>
       <c r="M16" s="1">
         <v>0.0</v>
       </c>
-      <c r="N16" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N16" s="2"/>
       <c r="O16" s="1">
         <v>0</v>
       </c>
@@ -6921,7 +6874,7 @@
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="1">
@@ -6972,15 +6925,11 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L17" s="2"/>
       <c r="M17" s="1">
         <v>0.0</v>
       </c>
-      <c r="N17" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N17" s="2"/>
       <c r="O17" s="1">
         <v>0</v>
       </c>
@@ -6989,7 +6938,7 @@
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="1">
@@ -7040,15 +6989,11 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L18" s="2"/>
       <c r="M18" s="1">
         <v>0.0</v>
       </c>
-      <c r="N18" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N18" s="2"/>
       <c r="O18" s="1">
         <v>0</v>
       </c>
@@ -7057,7 +7002,7 @@
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="1">
@@ -7108,15 +7053,11 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L19" s="2"/>
       <c r="M19" s="1">
         <v>0.0</v>
       </c>
-      <c r="N19" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N19" s="2"/>
       <c r="O19" s="1">
         <v>0</v>
       </c>
@@ -7125,7 +7066,7 @@
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S19" s="2"/>
       <c r="T19" s="1">
@@ -7176,15 +7117,11 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L20" s="2"/>
       <c r="M20" s="1">
         <v>0.0</v>
       </c>
-      <c r="N20" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N20" s="2"/>
       <c r="O20" s="1">
         <v>0</v>
       </c>
@@ -7193,7 +7130,7 @@
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="1">
@@ -7244,15 +7181,11 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L21" s="2"/>
       <c r="M21" s="1">
         <v>0.0</v>
       </c>
-      <c r="N21" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N21" s="2"/>
       <c r="O21" s="1">
         <v>0</v>
       </c>
@@ -7261,7 +7194,7 @@
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="1">
@@ -7312,15 +7245,11 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L22" s="2"/>
       <c r="M22" s="1">
         <v>0.0</v>
       </c>
-      <c r="N22" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N22" s="2"/>
       <c r="O22" s="1">
         <v>0</v>
       </c>
@@ -7329,7 +7258,7 @@
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S22" s="2"/>
       <c r="T22" s="1">
@@ -7380,15 +7309,11 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L23" s="2"/>
       <c r="M23" s="1">
         <v>0.0</v>
       </c>
-      <c r="N23" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N23" s="2"/>
       <c r="O23" s="1">
         <v>0</v>
       </c>
@@ -7397,7 +7322,7 @@
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S23" s="2"/>
       <c r="T23" s="1">
@@ -7448,15 +7373,11 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L24" s="2"/>
       <c r="M24" s="1">
         <v>0.0</v>
       </c>
-      <c r="N24" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N24" s="2"/>
       <c r="O24" s="1">
         <v>0</v>
       </c>
@@ -7465,7 +7386,7 @@
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="1">
@@ -7516,15 +7437,11 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L25" s="2"/>
       <c r="M25" s="1">
         <v>0.0</v>
       </c>
-      <c r="N25" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N25" s="2"/>
       <c r="O25" s="1">
         <v>0</v>
       </c>
@@ -7533,7 +7450,7 @@
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S25" s="2"/>
       <c r="T25" s="1">
@@ -7584,15 +7501,11 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-      <c r="L26" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L26" s="2"/>
       <c r="M26" s="1">
         <v>0.0</v>
       </c>
-      <c r="N26" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N26" s="2"/>
       <c r="O26" s="1">
         <v>0</v>
       </c>
@@ -7601,7 +7514,7 @@
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S26" s="2"/>
       <c r="T26" s="1">
@@ -7652,15 +7565,11 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-      <c r="L27" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L27" s="2"/>
       <c r="M27" s="1">
         <v>0.0</v>
       </c>
-      <c r="N27" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N27" s="2"/>
       <c r="O27" s="1">
         <v>0</v>
       </c>
@@ -7669,7 +7578,7 @@
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S27" s="2"/>
       <c r="T27" s="1">
@@ -7720,15 +7629,11 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-      <c r="L28" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L28" s="2"/>
       <c r="M28" s="1">
         <v>0.0</v>
       </c>
-      <c r="N28" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N28" s="2"/>
       <c r="O28" s="1">
         <v>0</v>
       </c>
@@ -7737,7 +7642,7 @@
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="1">
@@ -7788,15 +7693,11 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-      <c r="L29" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L29" s="2"/>
       <c r="M29" s="1">
         <v>0.0</v>
       </c>
-      <c r="N29" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N29" s="2"/>
       <c r="O29" s="1">
         <v>0</v>
       </c>
@@ -7805,7 +7706,7 @@
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S29" s="2"/>
       <c r="T29" s="1">
@@ -7856,15 +7757,11 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L30" s="2"/>
       <c r="M30" s="1">
         <v>0.0</v>
       </c>
-      <c r="N30" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N30" s="2"/>
       <c r="O30" s="1">
         <v>0</v>
       </c>
@@ -7873,7 +7770,7 @@
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S30" s="2"/>
       <c r="T30" s="1">
@@ -7924,15 +7821,11 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L31" s="2"/>
       <c r="M31" s="1">
         <v>0.0</v>
       </c>
-      <c r="N31" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N31" s="2"/>
       <c r="O31" s="1">
         <v>0</v>
       </c>
@@ -7941,7 +7834,7 @@
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S31" s="2"/>
       <c r="T31" s="1">
@@ -7992,15 +7885,11 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="L32" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L32" s="2"/>
       <c r="M32" s="1">
         <v>0.0</v>
       </c>
-      <c r="N32" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N32" s="2"/>
       <c r="O32" s="1">
         <v>0</v>
       </c>
@@ -8009,7 +7898,7 @@
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S32" s="2"/>
       <c r="T32" s="1">
@@ -8060,15 +7949,11 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L33" s="2"/>
       <c r="M33" s="1">
         <v>0.0</v>
       </c>
-      <c r="N33" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N33" s="2"/>
       <c r="O33" s="1">
         <v>0</v>
       </c>
@@ -8077,7 +7962,7 @@
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S33" s="2"/>
       <c r="T33" s="1">
@@ -8128,15 +8013,11 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L34" s="2"/>
       <c r="M34" s="1">
         <v>0.0</v>
       </c>
-      <c r="N34" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N34" s="2"/>
       <c r="O34" s="1">
         <v>0</v>
       </c>
@@ -8145,7 +8026,7 @@
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S34" s="2"/>
       <c r="T34" s="1">
@@ -8196,15 +8077,11 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="L35" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L35" s="2"/>
       <c r="M35" s="1">
         <v>0.0</v>
       </c>
-      <c r="N35" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N35" s="2"/>
       <c r="O35" s="1">
         <v>0</v>
       </c>
@@ -8213,7 +8090,7 @@
       </c>
       <c r="Q35" s="2"/>
       <c r="R35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S35" s="2"/>
       <c r="T35" s="1">
@@ -8264,15 +8141,11 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="L36" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L36" s="2"/>
       <c r="M36" s="1">
         <v>0.0</v>
       </c>
-      <c r="N36" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N36" s="2"/>
       <c r="O36" s="1">
         <v>0</v>
       </c>
@@ -8281,7 +8154,7 @@
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S36" s="2"/>
       <c r="T36" s="1">
@@ -8332,15 +8205,11 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="L37" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L37" s="2"/>
       <c r="M37" s="1">
         <v>0.0</v>
       </c>
-      <c r="N37" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N37" s="2"/>
       <c r="O37" s="1">
         <v>0</v>
       </c>
@@ -8349,7 +8218,7 @@
       </c>
       <c r="Q37" s="2"/>
       <c r="R37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S37" s="2"/>
       <c r="T37" s="1">
@@ -8400,15 +8269,11 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="L38" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L38" s="2"/>
       <c r="M38" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N38" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N38" s="2"/>
       <c r="O38" s="1">
         <v>0</v>
       </c>
@@ -8417,14 +8282,14 @@
       </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S38" s="2"/>
       <c r="T38" s="1">
         <v>0.0</v>
       </c>
       <c r="U38" s="6">
-        <v>60000.0</v>
+        <v>300000.0</v>
       </c>
       <c r="V38" s="1">
         <v>0.0</v>
@@ -8441,7 +8306,7 @@
         <v>0.0</v>
       </c>
       <c r="AB38">
-        <v>60000.0</v>
+        <v>300000.0</v>
       </c>
       <c r="AC38" s="2"/>
       <c r="AD38" t="s">
@@ -8456,7 +8321,7 @@
         <v>49</v>
       </c>
       <c r="C39" s="8">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="8">
@@ -8468,15 +8333,11 @@
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
-      <c r="L39" s="9">
-        <v>0.5</v>
-      </c>
+      <c r="L39" s="9"/>
       <c r="M39" s="8">
-        <v>-240000.0</v>
-      </c>
-      <c r="N39" s="9">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N39" s="9"/>
       <c r="O39" s="8">
         <v>0</v>
       </c>
@@ -8485,31 +8346,31 @@
       </c>
       <c r="Q39" s="9"/>
       <c r="R39" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S39" s="9"/>
       <c r="T39" s="8">
         <v>0.0</v>
       </c>
       <c r="U39" s="8">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V39" s="8">
         <v>0.0</v>
       </c>
       <c r="W39" s="9"/>
       <c r="X39" s="8">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y39" s="8">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z39" s="8"/>
       <c r="AA39" s="7">
         <v>0.0</v>
       </c>
       <c r="AB39" s="7">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC39" s="9"/>
       <c r="AD39" s="7" t="s">
@@ -8524,7 +8385,7 @@
         <v>50</v>
       </c>
       <c r="C40" s="11">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="11">
@@ -8536,15 +8397,11 @@
       <c r="I40" s="11"/>
       <c r="J40" s="11"/>
       <c r="K40" s="11"/>
-      <c r="L40" s="12">
-        <v>0.5</v>
-      </c>
+      <c r="L40" s="12"/>
       <c r="M40" s="11">
-        <v>-240000.0</v>
-      </c>
-      <c r="N40" s="12">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N40" s="12"/>
       <c r="O40" s="11">
         <v>0</v>
       </c>
@@ -8553,31 +8410,31 @@
       </c>
       <c r="Q40" s="12"/>
       <c r="R40" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S40" s="12"/>
       <c r="T40" s="11">
         <v>0.0</v>
       </c>
       <c r="U40" s="11">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V40" s="11">
         <v>0.0</v>
       </c>
       <c r="W40" s="12"/>
       <c r="X40" s="11">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y40" s="11">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z40" s="11"/>
       <c r="AA40" s="10">
         <v>0.0</v>
       </c>
       <c r="AB40" s="10">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC40" s="12"/>
       <c r="AD40" s="10" t="s">
@@ -8592,7 +8449,7 @@
         <v>51</v>
       </c>
       <c r="C41" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="5">
@@ -8604,15 +8461,11 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
-      <c r="L41" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L41" s="2"/>
       <c r="M41" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N41" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N41" s="2"/>
       <c r="O41" s="1">
         <v>0</v>
       </c>
@@ -8621,31 +8474,31 @@
       </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S41" s="2"/>
       <c r="T41" s="1">
         <v>0.0</v>
       </c>
       <c r="U41" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V41" s="1">
         <v>0.0</v>
       </c>
       <c r="W41" s="2"/>
       <c r="X41" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y41" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z41" s="1"/>
       <c r="AA41">
         <v>0.0</v>
       </c>
       <c r="AB41">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC41" s="2"/>
       <c r="AD41" t="s">
@@ -8660,7 +8513,7 @@
         <v>52</v>
       </c>
       <c r="C42" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="5">
@@ -8672,15 +8525,11 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L42" s="2"/>
       <c r="M42" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N42" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N42" s="2"/>
       <c r="O42" s="1">
         <v>0</v>
       </c>
@@ -8689,31 +8538,31 @@
       </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S42" s="2"/>
       <c r="T42" s="1">
         <v>0.0</v>
       </c>
       <c r="U42" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V42" s="1">
         <v>0.0</v>
       </c>
       <c r="W42" s="2"/>
       <c r="X42" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y42" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z42" s="1"/>
       <c r="AA42">
         <v>0.0</v>
       </c>
       <c r="AB42">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC42" s="2"/>
       <c r="AD42" t="s">
@@ -8728,7 +8577,7 @@
         <v>53</v>
       </c>
       <c r="C43" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="5">
@@ -8740,15 +8589,11 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L43" s="2"/>
       <c r="M43" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N43" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" s="1">
         <v>0</v>
       </c>
@@ -8757,31 +8602,31 @@
       </c>
       <c r="Q43" s="2"/>
       <c r="R43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S43" s="2"/>
       <c r="T43" s="1">
         <v>0.0</v>
       </c>
       <c r="U43" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V43" s="1">
         <v>0.0</v>
       </c>
       <c r="W43" s="2"/>
       <c r="X43" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y43" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z43" s="1"/>
       <c r="AA43">
         <v>0.0</v>
       </c>
       <c r="AB43">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC43" s="2"/>
       <c r="AD43" t="s">
@@ -8796,7 +8641,7 @@
         <v>54</v>
       </c>
       <c r="C44" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="5">
@@ -8808,15 +8653,11 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="L44" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L44" s="2"/>
       <c r="M44" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N44" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N44" s="2"/>
       <c r="O44" s="1">
         <v>0</v>
       </c>
@@ -8825,31 +8666,31 @@
       </c>
       <c r="Q44" s="2"/>
       <c r="R44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S44" s="2"/>
       <c r="T44" s="1">
         <v>0.0</v>
       </c>
       <c r="U44" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V44" s="1">
         <v>0.0</v>
       </c>
       <c r="W44" s="2"/>
       <c r="X44" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y44" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z44" s="1"/>
       <c r="AA44">
         <v>0.0</v>
       </c>
       <c r="AB44">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC44" s="2"/>
       <c r="AD44" t="s">
@@ -8864,7 +8705,7 @@
         <v>55</v>
       </c>
       <c r="C45" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5">
@@ -8876,15 +8717,11 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
-      <c r="L45" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L45" s="2"/>
       <c r="M45" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N45" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N45" s="2"/>
       <c r="O45" s="1">
         <v>0</v>
       </c>
@@ -8893,31 +8730,31 @@
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S45" s="2"/>
       <c r="T45" s="1">
         <v>0.0</v>
       </c>
       <c r="U45" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V45" s="1">
         <v>0.0</v>
       </c>
       <c r="W45" s="2"/>
       <c r="X45" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y45" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z45" s="1"/>
       <c r="AA45">
         <v>0.0</v>
       </c>
       <c r="AB45">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC45" s="2"/>
       <c r="AD45" t="s">
@@ -8932,7 +8769,7 @@
         <v>56</v>
       </c>
       <c r="C46" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="5">
@@ -8944,15 +8781,11 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L46" s="2"/>
       <c r="M46" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N46" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" s="1">
         <v>0</v>
       </c>
@@ -8961,31 +8794,31 @@
       </c>
       <c r="Q46" s="2"/>
       <c r="R46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S46" s="2"/>
       <c r="T46" s="1">
         <v>0.0</v>
       </c>
       <c r="U46" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V46" s="1">
         <v>0.0</v>
       </c>
       <c r="W46" s="2"/>
       <c r="X46" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y46" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z46" s="1"/>
       <c r="AA46">
         <v>0.0</v>
       </c>
       <c r="AB46">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC46" s="2"/>
       <c r="AD46" t="s">
@@ -9000,7 +8833,7 @@
         <v>57</v>
       </c>
       <c r="C47" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5">
@@ -9012,15 +8845,11 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
-      <c r="L47" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L47" s="2"/>
       <c r="M47" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N47" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N47" s="2"/>
       <c r="O47" s="1">
         <v>0</v>
       </c>
@@ -9029,31 +8858,31 @@
       </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S47" s="2"/>
       <c r="T47" s="1">
         <v>0.0</v>
       </c>
       <c r="U47" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V47" s="1">
         <v>0.0</v>
       </c>
       <c r="W47" s="2"/>
       <c r="X47" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y47" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z47" s="1"/>
       <c r="AA47">
         <v>0.0</v>
       </c>
       <c r="AB47">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC47" s="2"/>
       <c r="AD47" t="s">
@@ -9068,7 +8897,7 @@
         <v>58</v>
       </c>
       <c r="C48" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="5">
@@ -9080,15 +8909,11 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="L48" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L48" s="2"/>
       <c r="M48" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N48" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N48" s="2"/>
       <c r="O48" s="1">
         <v>0</v>
       </c>
@@ -9097,31 +8922,31 @@
       </c>
       <c r="Q48" s="2"/>
       <c r="R48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S48" s="2"/>
       <c r="T48" s="1">
         <v>0.0</v>
       </c>
       <c r="U48" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V48" s="1">
         <v>0.0</v>
       </c>
       <c r="W48" s="2"/>
       <c r="X48" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y48" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z48" s="1"/>
       <c r="AA48">
         <v>0.0</v>
       </c>
       <c r="AB48">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC48" s="2"/>
       <c r="AD48" t="s">
@@ -9136,7 +8961,7 @@
         <v>59</v>
       </c>
       <c r="C49" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="5">
@@ -9148,15 +8973,11 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-      <c r="L49" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L49" s="2"/>
       <c r="M49" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N49" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N49" s="2"/>
       <c r="O49" s="1">
         <v>0</v>
       </c>
@@ -9165,31 +8986,31 @@
       </c>
       <c r="Q49" s="2"/>
       <c r="R49" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S49" s="2"/>
       <c r="T49" s="1">
         <v>0.0</v>
       </c>
       <c r="U49" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V49" s="1">
         <v>0.0</v>
       </c>
       <c r="W49" s="2"/>
       <c r="X49" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y49" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z49" s="1"/>
       <c r="AA49">
         <v>0.0</v>
       </c>
       <c r="AB49">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC49" s="2"/>
       <c r="AD49" t="s">
@@ -9204,7 +9025,7 @@
         <v>60</v>
       </c>
       <c r="C50" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="5">
@@ -9216,15 +9037,11 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
-      <c r="L50" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L50" s="2"/>
       <c r="M50" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N50" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N50" s="2"/>
       <c r="O50" s="1">
         <v>0</v>
       </c>
@@ -9233,31 +9050,31 @@
       </c>
       <c r="Q50" s="2"/>
       <c r="R50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S50" s="2"/>
       <c r="T50" s="1">
         <v>0.0</v>
       </c>
       <c r="U50" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V50" s="1">
         <v>0.0</v>
       </c>
       <c r="W50" s="2"/>
       <c r="X50" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y50" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z50" s="1"/>
       <c r="AA50">
         <v>0.0</v>
       </c>
       <c r="AB50">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC50" s="2"/>
       <c r="AD50" t="s">
@@ -9272,7 +9089,7 @@
         <v>61</v>
       </c>
       <c r="C51" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="5">
@@ -9284,15 +9101,11 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
-      <c r="L51" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L51" s="2"/>
       <c r="M51" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N51" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N51" s="2"/>
       <c r="O51" s="1">
         <v>0</v>
       </c>
@@ -9301,31 +9114,31 @@
       </c>
       <c r="Q51" s="2"/>
       <c r="R51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S51" s="2"/>
       <c r="T51" s="1">
         <v>0.0</v>
       </c>
       <c r="U51" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V51" s="1">
         <v>0.0</v>
       </c>
       <c r="W51" s="2"/>
       <c r="X51" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y51" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z51" s="1"/>
       <c r="AA51">
         <v>0.0</v>
       </c>
       <c r="AB51">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC51" s="2"/>
       <c r="AD51" t="s">
@@ -9340,7 +9153,7 @@
         <v>62</v>
       </c>
       <c r="C52" s="4">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="5">
@@ -9352,15 +9165,11 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="L52" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L52" s="2"/>
       <c r="M52" s="1">
-        <v>-240000.0</v>
-      </c>
-      <c r="N52" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="N52" s="2"/>
       <c r="O52" s="1">
         <v>0</v>
       </c>
@@ -9369,31 +9178,31 @@
       </c>
       <c r="Q52" s="2"/>
       <c r="R52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S52" s="2"/>
       <c r="T52" s="1">
         <v>0.0</v>
       </c>
       <c r="U52" s="6">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="V52" s="1">
         <v>0.0</v>
       </c>
       <c r="W52" s="2"/>
       <c r="X52" s="1">
-        <v>480000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y52" s="1">
-        <v>2400000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Z52" s="1"/>
       <c r="AA52">
         <v>0.0</v>
       </c>
       <c r="AB52">
-        <v>60000.0</v>
+        <v>-180000.0</v>
       </c>
       <c r="AC52" s="2"/>
       <c r="AD52" t="s">
@@ -9420,15 +9229,11 @@
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
       <c r="K53" s="13"/>
-      <c r="L53" s="14">
-        <v>0.5</v>
-      </c>
+      <c r="L53" s="14"/>
       <c r="M53" s="13">
         <v>0.0</v>
       </c>
-      <c r="N53" s="14">
-        <v>0.5</v>
-      </c>
+      <c r="N53" s="14"/>
       <c r="O53" s="13">
         <v>0</v>
       </c>
@@ -9437,7 +9242,7 @@
       </c>
       <c r="Q53" s="14"/>
       <c r="R53" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S53" s="14"/>
       <c r="T53" s="13">
@@ -9488,15 +9293,11 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-      <c r="L54" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L54" s="2"/>
       <c r="M54" s="1">
         <v>0.0</v>
       </c>
-      <c r="N54" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N54" s="2"/>
       <c r="O54" s="1">
         <v>0</v>
       </c>
@@ -9505,7 +9306,7 @@
       </c>
       <c r="Q54" s="2"/>
       <c r="R54" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S54" s="2"/>
       <c r="T54" s="1">
@@ -9533,7 +9334,7 @@
       </c>
       <c r="AC54" s="2"/>
       <c r="AD54" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:31">
@@ -9556,15 +9357,11 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
-      <c r="L55" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L55" s="2"/>
       <c r="M55" s="1">
         <v>0.0</v>
       </c>
-      <c r="N55" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N55" s="2"/>
       <c r="O55" s="1">
         <v>0</v>
       </c>
@@ -9573,7 +9370,7 @@
       </c>
       <c r="Q55" s="2"/>
       <c r="R55" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S55" s="2"/>
       <c r="T55" s="1">
@@ -9601,7 +9398,7 @@
       </c>
       <c r="AC55" s="2"/>
       <c r="AD55" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:31">
@@ -9624,15 +9421,11 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
-      <c r="L56" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L56" s="2"/>
       <c r="M56" s="1">
         <v>0.0</v>
       </c>
-      <c r="N56" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N56" s="2"/>
       <c r="O56" s="1">
         <v>0</v>
       </c>
@@ -9641,7 +9434,7 @@
       </c>
       <c r="Q56" s="2"/>
       <c r="R56" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S56" s="2"/>
       <c r="T56" s="1">
@@ -9669,7 +9462,7 @@
       </c>
       <c r="AC56" s="2"/>
       <c r="AD56" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:31">
@@ -9692,15 +9485,11 @@
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
-      <c r="L57" s="14">
-        <v>0.5</v>
-      </c>
+      <c r="L57" s="14"/>
       <c r="M57" s="13">
         <v>0.0</v>
       </c>
-      <c r="N57" s="14">
-        <v>0.5</v>
-      </c>
+      <c r="N57" s="14"/>
       <c r="O57" s="13">
         <v>0</v>
       </c>
@@ -9709,7 +9498,7 @@
       </c>
       <c r="Q57" s="14"/>
       <c r="R57" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S57" s="14"/>
       <c r="T57" s="13">
@@ -9737,7 +9526,7 @@
       </c>
       <c r="AC57" s="14"/>
       <c r="AD57" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:31">
@@ -9760,15 +9549,11 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
-      <c r="L58" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L58" s="2"/>
       <c r="M58" s="1">
         <v>0.0</v>
       </c>
-      <c r="N58" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N58" s="2"/>
       <c r="O58" s="1">
         <v>0</v>
       </c>
@@ -9777,7 +9562,7 @@
       </c>
       <c r="Q58" s="2"/>
       <c r="R58" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S58" s="2"/>
       <c r="T58" s="1">
@@ -9805,7 +9590,7 @@
       </c>
       <c r="AC58" s="2"/>
       <c r="AD58" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:31">
@@ -9828,15 +9613,11 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
-      <c r="L59" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L59" s="2"/>
       <c r="M59" s="1">
         <v>0.0</v>
       </c>
-      <c r="N59" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N59" s="2"/>
       <c r="O59" s="1">
         <v>0</v>
       </c>
@@ -9845,7 +9626,7 @@
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S59" s="2"/>
       <c r="T59" s="1">
@@ -9873,7 +9654,7 @@
       </c>
       <c r="AC59" s="2"/>
       <c r="AD59" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:31">
@@ -9896,15 +9677,11 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
-      <c r="L60" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L60" s="2"/>
       <c r="M60" s="1">
         <v>0.0</v>
       </c>
-      <c r="N60" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N60" s="2"/>
       <c r="O60" s="1">
         <v>0</v>
       </c>
@@ -9913,7 +9690,7 @@
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S60" s="2"/>
       <c r="T60" s="1">
@@ -9941,7 +9718,7 @@
       </c>
       <c r="AC60" s="2"/>
       <c r="AD60" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:31">
@@ -9964,15 +9741,11 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
-      <c r="L61" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L61" s="2"/>
       <c r="M61" s="1">
         <v>0.0</v>
       </c>
-      <c r="N61" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N61" s="2"/>
       <c r="O61" s="1">
         <v>0</v>
       </c>
@@ -9981,7 +9754,7 @@
       </c>
       <c r="Q61" s="2"/>
       <c r="R61" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S61" s="2"/>
       <c r="T61" s="1">
@@ -10009,7 +9782,7 @@
       </c>
       <c r="AC61" s="2"/>
       <c r="AD61" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:31">
@@ -10032,15 +9805,11 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
-      <c r="L62" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L62" s="2"/>
       <c r="M62" s="1">
         <v>0.0</v>
       </c>
-      <c r="N62" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N62" s="2"/>
       <c r="O62" s="1">
         <v>0</v>
       </c>
@@ -10049,7 +9818,7 @@
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S62" s="2"/>
       <c r="T62" s="1">
@@ -10077,7 +9846,7 @@
       </c>
       <c r="AC62" s="2"/>
       <c r="AD62" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:31">
@@ -10100,15 +9869,11 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
-      <c r="L63" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L63" s="2"/>
       <c r="M63" s="1">
         <v>0.0</v>
       </c>
-      <c r="N63" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N63" s="2"/>
       <c r="O63" s="1">
         <v>0</v>
       </c>
@@ -10117,7 +9882,7 @@
       </c>
       <c r="Q63" s="2"/>
       <c r="R63" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S63" s="2"/>
       <c r="T63" s="1">
@@ -10145,7 +9910,7 @@
       </c>
       <c r="AC63" s="2"/>
       <c r="AD63" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:31">
@@ -10168,15 +9933,11 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
-      <c r="L64" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L64" s="2"/>
       <c r="M64" s="1">
         <v>0.0</v>
       </c>
-      <c r="N64" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N64" s="2"/>
       <c r="O64" s="1">
         <v>0</v>
       </c>
@@ -10185,7 +9946,7 @@
       </c>
       <c r="Q64" s="2"/>
       <c r="R64" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S64" s="2"/>
       <c r="T64" s="1">
@@ -10213,7 +9974,7 @@
       </c>
       <c r="AC64" s="2"/>
       <c r="AD64" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:31">
@@ -10236,15 +9997,11 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
-      <c r="L65" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L65" s="2"/>
       <c r="M65" s="1">
         <v>0.0</v>
       </c>
-      <c r="N65" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N65" s="2"/>
       <c r="O65" s="1">
         <v>0</v>
       </c>
@@ -10253,7 +10010,7 @@
       </c>
       <c r="Q65" s="2"/>
       <c r="R65" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S65" s="2"/>
       <c r="T65" s="1">
@@ -10281,7 +10038,7 @@
       </c>
       <c r="AC65" s="2"/>
       <c r="AD65" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:31">
@@ -10304,15 +10061,11 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
-      <c r="L66" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L66" s="2"/>
       <c r="M66" s="1">
         <v>0.0</v>
       </c>
-      <c r="N66" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N66" s="2"/>
       <c r="O66" s="1">
         <v>0</v>
       </c>
@@ -10321,7 +10074,7 @@
       </c>
       <c r="Q66" s="2"/>
       <c r="R66" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S66" s="2"/>
       <c r="T66" s="1">
@@ -10349,7 +10102,7 @@
       </c>
       <c r="AC66" s="2"/>
       <c r="AD66" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:31">
@@ -10372,15 +10125,11 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
-      <c r="L67" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L67" s="2"/>
       <c r="M67" s="1">
         <v>0.0</v>
       </c>
-      <c r="N67" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N67" s="2"/>
       <c r="O67" s="1">
         <v>0</v>
       </c>
@@ -10389,7 +10138,7 @@
       </c>
       <c r="Q67" s="2"/>
       <c r="R67" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S67" s="2"/>
       <c r="T67" s="1">
@@ -10417,7 +10166,7 @@
       </c>
       <c r="AC67" s="2"/>
       <c r="AD67" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:31">
@@ -10440,15 +10189,11 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
-      <c r="L68" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L68" s="2"/>
       <c r="M68" s="1">
         <v>0.0</v>
       </c>
-      <c r="N68" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N68" s="2"/>
       <c r="O68" s="1">
         <v>0</v>
       </c>
@@ -10457,7 +10202,7 @@
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S68" s="2"/>
       <c r="T68" s="1">
@@ -10485,7 +10230,7 @@
       </c>
       <c r="AC68" s="2"/>
       <c r="AD68" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:31">
@@ -10508,15 +10253,11 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
-      <c r="L69" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L69" s="2"/>
       <c r="M69" s="1">
         <v>0.0</v>
       </c>
-      <c r="N69" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N69" s="2"/>
       <c r="O69" s="1">
         <v>0</v>
       </c>
@@ -10525,7 +10266,7 @@
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S69" s="2"/>
       <c r="T69" s="1">
@@ -10553,7 +10294,7 @@
       </c>
       <c r="AC69" s="2"/>
       <c r="AD69" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:31">
@@ -10576,15 +10317,11 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
-      <c r="L70" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L70" s="2"/>
       <c r="M70" s="1">
         <v>0.0</v>
       </c>
-      <c r="N70" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N70" s="2"/>
       <c r="O70" s="1">
         <v>0</v>
       </c>
@@ -10593,7 +10330,7 @@
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S70" s="2"/>
       <c r="T70" s="1">
@@ -10621,7 +10358,7 @@
       </c>
       <c r="AC70" s="2"/>
       <c r="AD70" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:31">
@@ -10644,15 +10381,11 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
-      <c r="L71" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L71" s="2"/>
       <c r="M71" s="1">
         <v>0.0</v>
       </c>
-      <c r="N71" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N71" s="2"/>
       <c r="O71" s="1">
         <v>0</v>
       </c>
@@ -10661,7 +10394,7 @@
       </c>
       <c r="Q71" s="2"/>
       <c r="R71" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S71" s="2"/>
       <c r="T71" s="1">
@@ -10689,7 +10422,7 @@
       </c>
       <c r="AC71" s="2"/>
       <c r="AD71" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:31">
@@ -10712,15 +10445,11 @@
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
-      <c r="L72" s="16">
-        <v>0.5</v>
-      </c>
+      <c r="L72" s="16"/>
       <c r="M72" s="5">
         <v>0.0</v>
       </c>
-      <c r="N72" s="16">
-        <v>0.5</v>
-      </c>
+      <c r="N72" s="16"/>
       <c r="O72" s="5">
         <v>0</v>
       </c>
@@ -10729,7 +10458,7 @@
       </c>
       <c r="Q72" s="16"/>
       <c r="R72" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S72" s="16"/>
       <c r="T72" s="5">
@@ -10757,7 +10486,7 @@
       </c>
       <c r="AC72" s="16"/>
       <c r="AD72" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:31">
@@ -11043,7 +10772,7 @@
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:31">
@@ -11051,7 +10780,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -11063,7 +10792,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -13358,7 +13087,7 @@
       </c>
       <c r="AC39" s="9"/>
       <c r="AD39" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:31">
@@ -13424,7 +13153,7 @@
       </c>
       <c r="AC40" s="12"/>
       <c r="AD40" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:31">
@@ -13490,7 +13219,7 @@
       </c>
       <c r="AC41" s="2"/>
       <c r="AD41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:31">
@@ -13556,7 +13285,7 @@
       </c>
       <c r="AC42" s="2"/>
       <c r="AD42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:31">
@@ -13622,7 +13351,7 @@
       </c>
       <c r="AC43" s="2"/>
       <c r="AD43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:31">
@@ -13688,7 +13417,7 @@
       </c>
       <c r="AC44" s="2"/>
       <c r="AD44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:31">
@@ -13754,7 +13483,7 @@
       </c>
       <c r="AC45" s="2"/>
       <c r="AD45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:31">
@@ -13820,7 +13549,7 @@
       </c>
       <c r="AC46" s="2"/>
       <c r="AD46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:31">
@@ -13886,7 +13615,7 @@
       </c>
       <c r="AC47" s="2"/>
       <c r="AD47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:31">
@@ -13952,7 +13681,7 @@
       </c>
       <c r="AC48" s="2"/>
       <c r="AD48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:31">
@@ -14018,7 +13747,7 @@
       </c>
       <c r="AC49" s="2"/>
       <c r="AD49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:31">
@@ -14084,7 +13813,7 @@
       </c>
       <c r="AC50" s="2"/>
       <c r="AD50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:31">
@@ -14150,7 +13879,7 @@
       </c>
       <c r="AC51" s="2"/>
       <c r="AD51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:31">
@@ -14216,7 +13945,7 @@
       </c>
       <c r="AC52" s="2"/>
       <c r="AD52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:31">
@@ -14282,7 +14011,7 @@
       </c>
       <c r="AC53" s="14"/>
       <c r="AD53" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:31">
@@ -14348,7 +14077,7 @@
       </c>
       <c r="AC54" s="2"/>
       <c r="AD54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:31">
@@ -14414,7 +14143,7 @@
       </c>
       <c r="AC55" s="2"/>
       <c r="AD55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:31">
@@ -14480,7 +14209,7 @@
       </c>
       <c r="AC56" s="2"/>
       <c r="AD56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:31">
@@ -14546,7 +14275,7 @@
       </c>
       <c r="AC57" s="14"/>
       <c r="AD57" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:31">
@@ -14612,7 +14341,7 @@
       </c>
       <c r="AC58" s="2"/>
       <c r="AD58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:31">
@@ -14678,7 +14407,7 @@
       </c>
       <c r="AC59" s="2"/>
       <c r="AD59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:31">
@@ -14744,7 +14473,7 @@
       </c>
       <c r="AC60" s="2"/>
       <c r="AD60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:31">
@@ -14810,7 +14539,7 @@
       </c>
       <c r="AC61" s="2"/>
       <c r="AD61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:31">
@@ -14876,7 +14605,7 @@
       </c>
       <c r="AC62" s="2"/>
       <c r="AD62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:31">
@@ -14942,7 +14671,7 @@
       </c>
       <c r="AC63" s="2"/>
       <c r="AD63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:31">
@@ -15008,7 +14737,7 @@
       </c>
       <c r="AC64" s="2"/>
       <c r="AD64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:31">
@@ -15074,7 +14803,7 @@
       </c>
       <c r="AC65" s="2"/>
       <c r="AD65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:31">
@@ -15140,7 +14869,7 @@
       </c>
       <c r="AC66" s="2"/>
       <c r="AD66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:31">
@@ -15206,7 +14935,7 @@
       </c>
       <c r="AC67" s="2"/>
       <c r="AD67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:31">
@@ -15272,7 +15001,7 @@
       </c>
       <c r="AC68" s="2"/>
       <c r="AD68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:31">
@@ -15338,7 +15067,7 @@
       </c>
       <c r="AC69" s="2"/>
       <c r="AD69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:31">
@@ -15404,7 +15133,7 @@
       </c>
       <c r="AC70" s="2"/>
       <c r="AD70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:31">
@@ -15470,7 +15199,7 @@
       </c>
       <c r="AC71" s="2"/>
       <c r="AD71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:31">
@@ -15534,7 +15263,7 @@
       </c>
       <c r="AC72" s="16"/>
       <c r="AD72" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:31">
@@ -15792,10 +15521,10 @@
   <sheetData>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
New config format updated and tested in all examples, refactored transfer of amounts from one asset to another, and sourcing of the amount on one asset to calculate a value to add to another asset
</commit_message>
<xml_diff>
--- a/tests/Feature/config/fond_zero.xlsx
+++ b/tests/Feature/config/fond_zero.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
   <si>
     <t>private</t>
   </si>
@@ -170,13 +170,64 @@
     <t>000 Asset rule Using current amount: 100000 * 1</t>
   </si>
   <si>
-    <t>00Uttak fra 2068, 1|3 Asset rule 1|2Adding divisor: 33333 new rule: 1|2</t>
+    <t>00Uttak fra 2068, 1|20 Asset rule 1|19Adding divisor: 5000 new rule: 1|19</t>
   </si>
   <si>
-    <t>000 Asset rule 1|1Adding divisor: 33334 new rule: 1|1</t>
+    <t>000 Asset rule 1|18Adding divisor: 5000 new rule: 1|18</t>
   </si>
   <si>
-    <t xml:space="preserve">000 Asset rule Adding divisor: 33333 new rule: </t>
+    <t>000 Asset rule 1|17Adding divisor: 5000 new rule: 1|17</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|16Adding divisor: 5000 new rule: 1|16</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|15Adding divisor: 5000 new rule: 1|15</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|14Adding divisor: 5000 new rule: 1|14</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|13Adding divisor: 5000 new rule: 1|13</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|12Adding divisor: 5000 new rule: 1|12</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|11Adding divisor: 5000 new rule: 1|11</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|10Adding divisor: 5000 new rule: 1|10</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|9Adding divisor: 5000 new rule: 1|9</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|8Adding divisor: 5000 new rule: 1|8</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|7Adding divisor: 5000 new rule: 1|7</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|6Adding divisor: 5000 new rule: 1|6</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|5Adding divisor: 5000 new rule: 1|5</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|4Adding divisor: 5000 new rule: 1|4</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|3Adding divisor: 5000 new rule: 1|3</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|2Adding divisor: 5000 new rule: 1|2</t>
+  </si>
+  <si>
+    <t>000 Asset rule 1|1Adding divisor: 5000 new rule: 1|1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000 Asset rule Adding divisor: 5000 new rule: </t>
   </si>
   <si>
     <t>total</t>
@@ -4489,7 +4540,7 @@
         <v>63</v>
       </c>
       <c r="C53" s="13">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="13">
@@ -4518,20 +4569,20 @@
       </c>
       <c r="O53" s="14"/>
       <c r="P53" s="13">
-        <v>100000.0</v>
+        <v>95000.0</v>
       </c>
       <c r="Q53" s="14"/>
       <c r="R53" s="13">
-        <v>100000.0</v>
+        <v>95000.0</v>
       </c>
       <c r="S53" s="13">
         <v>100000.0</v>
       </c>
       <c r="T53" s="13">
-        <v>100000.0</v>
+        <v>95000.0</v>
       </c>
       <c r="U53" s="13">
-        <v>80000.0</v>
+        <v>76000.0</v>
       </c>
       <c r="V53" s="14"/>
       <c r="W53" s="13">
@@ -4556,7 +4607,7 @@
       </c>
       <c r="AE53" s="3"/>
       <c r="AF53" s="3">
-        <v>0.44</v>
+        <v>0.19</v>
       </c>
       <c r="AG53"/>
     </row>
@@ -4568,7 +4619,7 @@
         <v>64</v>
       </c>
       <c r="C54" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="5">
@@ -4597,20 +4648,20 @@
       </c>
       <c r="O54" s="2"/>
       <c r="P54" s="6">
-        <v>100000.0</v>
+        <v>90000.0</v>
       </c>
       <c r="Q54" s="2"/>
       <c r="R54" s="1">
-        <v>100000.0</v>
+        <v>90000.0</v>
       </c>
       <c r="S54" s="1">
         <v>100000.0</v>
       </c>
       <c r="T54" s="1">
-        <v>100000.0</v>
+        <v>90000.0</v>
       </c>
       <c r="U54" s="6">
-        <v>80000.0</v>
+        <v>72000.0</v>
       </c>
       <c r="V54" s="2"/>
       <c r="W54" s="1">
@@ -4635,7 +4686,7 @@
       </c>
       <c r="AE54"/>
       <c r="AF54">
-        <v>0.44</v>
+        <v>0.19</v>
       </c>
       <c r="AG54"/>
     </row>
@@ -4647,7 +4698,7 @@
         <v>65</v>
       </c>
       <c r="C55" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="5">
@@ -4676,20 +4727,20 @@
       </c>
       <c r="O55" s="2"/>
       <c r="P55" s="6">
-        <v>100000.0</v>
+        <v>85000.0</v>
       </c>
       <c r="Q55" s="2"/>
       <c r="R55" s="1">
-        <v>100000.0</v>
+        <v>85000.0</v>
       </c>
       <c r="S55" s="1">
         <v>100000.0</v>
       </c>
       <c r="T55" s="1">
-        <v>100000.0</v>
+        <v>85000.0</v>
       </c>
       <c r="U55" s="6">
-        <v>80000.0</v>
+        <v>68000.0</v>
       </c>
       <c r="V55" s="2"/>
       <c r="W55" s="1">
@@ -4714,7 +4765,7 @@
       </c>
       <c r="AE55"/>
       <c r="AF55">
-        <v>0.44</v>
+        <v>0.2</v>
       </c>
       <c r="AG55"/>
     </row>
@@ -4726,7 +4777,7 @@
         <v>66</v>
       </c>
       <c r="C56" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="5">
@@ -4755,20 +4806,20 @@
       </c>
       <c r="O56" s="2"/>
       <c r="P56" s="6">
-        <v>100000.0</v>
+        <v>80000.0</v>
       </c>
       <c r="Q56" s="2"/>
       <c r="R56" s="1">
-        <v>100000.0</v>
+        <v>80000.0</v>
       </c>
       <c r="S56" s="1">
         <v>100000.0</v>
       </c>
       <c r="T56" s="1">
-        <v>100000.0</v>
+        <v>80000.0</v>
       </c>
       <c r="U56" s="6">
-        <v>80000.0</v>
+        <v>64000.0</v>
       </c>
       <c r="V56" s="2"/>
       <c r="W56" s="1">
@@ -4793,7 +4844,7 @@
       </c>
       <c r="AE56"/>
       <c r="AF56">
-        <v>0.44</v>
+        <v>0.2</v>
       </c>
       <c r="AG56"/>
     </row>
@@ -4805,7 +4856,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="13">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="13">
@@ -4834,20 +4885,20 @@
       </c>
       <c r="O57" s="14"/>
       <c r="P57" s="13">
-        <v>100000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="Q57" s="14"/>
       <c r="R57" s="13">
-        <v>100000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="S57" s="13">
         <v>100000.0</v>
       </c>
       <c r="T57" s="13">
-        <v>100000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="U57" s="13">
-        <v>80000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="V57" s="14"/>
       <c r="W57" s="13">
@@ -4872,7 +4923,7 @@
       </c>
       <c r="AE57" s="3"/>
       <c r="AF57" s="3">
-        <v>0.44</v>
+        <v>0.21</v>
       </c>
       <c r="AG57"/>
     </row>
@@ -4884,7 +4935,7 @@
         <v>68</v>
       </c>
       <c r="C58" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="5">
@@ -4913,20 +4964,20 @@
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="6">
-        <v>100000.0</v>
+        <v>70000.0</v>
       </c>
       <c r="Q58" s="2"/>
       <c r="R58" s="1">
-        <v>100000.0</v>
+        <v>70000.0</v>
       </c>
       <c r="S58" s="1">
         <v>100000.0</v>
       </c>
       <c r="T58" s="1">
-        <v>100000.0</v>
+        <v>70000.0</v>
       </c>
       <c r="U58" s="6">
-        <v>80000.0</v>
+        <v>56000.0</v>
       </c>
       <c r="V58" s="2"/>
       <c r="W58" s="1">
@@ -4951,7 +5002,7 @@
       </c>
       <c r="AE58"/>
       <c r="AF58">
-        <v>0.44</v>
+        <v>0.22</v>
       </c>
       <c r="AG58"/>
     </row>
@@ -4963,7 +5014,7 @@
         <v>69</v>
       </c>
       <c r="C59" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="5">
@@ -4992,20 +5043,20 @@
       </c>
       <c r="O59" s="2"/>
       <c r="P59" s="6">
-        <v>100000.0</v>
+        <v>65000.0</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="1">
-        <v>100000.0</v>
+        <v>65000.0</v>
       </c>
       <c r="S59" s="1">
         <v>100000.0</v>
       </c>
       <c r="T59" s="1">
-        <v>100000.0</v>
+        <v>65000.0</v>
       </c>
       <c r="U59" s="6">
-        <v>80000.0</v>
+        <v>52000.0</v>
       </c>
       <c r="V59" s="2"/>
       <c r="W59" s="1">
@@ -5030,7 +5081,7 @@
       </c>
       <c r="AE59"/>
       <c r="AF59">
-        <v>0.44</v>
+        <v>0.22</v>
       </c>
       <c r="AG59"/>
     </row>
@@ -5042,7 +5093,7 @@
         <v>70</v>
       </c>
       <c r="C60" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="5">
@@ -5071,20 +5122,20 @@
       </c>
       <c r="O60" s="2"/>
       <c r="P60" s="6">
-        <v>100000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="1">
-        <v>100000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="S60" s="1">
         <v>100000.0</v>
       </c>
       <c r="T60" s="1">
-        <v>100000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="U60" s="6">
-        <v>80000.0</v>
+        <v>48000.0</v>
       </c>
       <c r="V60" s="2"/>
       <c r="W60" s="1">
@@ -5109,7 +5160,7 @@
       </c>
       <c r="AE60"/>
       <c r="AF60">
-        <v>0.44</v>
+        <v>0.23</v>
       </c>
       <c r="AG60"/>
     </row>
@@ -5121,7 +5172,7 @@
         <v>71</v>
       </c>
       <c r="C61" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="5">
@@ -5150,20 +5201,20 @@
       </c>
       <c r="O61" s="2"/>
       <c r="P61" s="6">
-        <v>100000.0</v>
+        <v>55000.0</v>
       </c>
       <c r="Q61" s="2"/>
       <c r="R61" s="1">
-        <v>100000.0</v>
+        <v>55000.0</v>
       </c>
       <c r="S61" s="1">
         <v>100000.0</v>
       </c>
       <c r="T61" s="1">
-        <v>100000.0</v>
+        <v>55000.0</v>
       </c>
       <c r="U61" s="6">
-        <v>80000.0</v>
+        <v>44000.0</v>
       </c>
       <c r="V61" s="2"/>
       <c r="W61" s="1">
@@ -5188,7 +5239,7 @@
       </c>
       <c r="AE61"/>
       <c r="AF61">
-        <v>0.44</v>
+        <v>0.24</v>
       </c>
       <c r="AG61"/>
     </row>
@@ -5200,7 +5251,7 @@
         <v>72</v>
       </c>
       <c r="C62" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="5">
@@ -5229,20 +5280,20 @@
       </c>
       <c r="O62" s="2"/>
       <c r="P62" s="6">
-        <v>100000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="1">
-        <v>100000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="S62" s="1">
         <v>100000.0</v>
       </c>
       <c r="T62" s="1">
-        <v>100000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="U62" s="6">
-        <v>80000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="V62" s="2"/>
       <c r="W62" s="1">
@@ -5267,7 +5318,7 @@
       </c>
       <c r="AE62"/>
       <c r="AF62">
-        <v>0.44</v>
+        <v>0.24</v>
       </c>
       <c r="AG62"/>
     </row>
@@ -5279,7 +5330,7 @@
         <v>73</v>
       </c>
       <c r="C63" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="5">
@@ -5308,20 +5359,20 @@
       </c>
       <c r="O63" s="2"/>
       <c r="P63" s="6">
-        <v>100000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="Q63" s="2"/>
       <c r="R63" s="1">
-        <v>100000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="S63" s="1">
         <v>100000.0</v>
       </c>
       <c r="T63" s="1">
-        <v>100000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="U63" s="6">
-        <v>80000.0</v>
+        <v>36000.0</v>
       </c>
       <c r="V63" s="2"/>
       <c r="W63" s="1">
@@ -5346,7 +5397,7 @@
       </c>
       <c r="AE63"/>
       <c r="AF63">
-        <v>0.44</v>
+        <v>0.25</v>
       </c>
       <c r="AG63"/>
     </row>
@@ -5358,7 +5409,7 @@
         <v>74</v>
       </c>
       <c r="C64" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="5">
@@ -5387,20 +5438,20 @@
       </c>
       <c r="O64" s="2"/>
       <c r="P64" s="6">
-        <v>100000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="Q64" s="2"/>
       <c r="R64" s="1">
-        <v>100000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="S64" s="1">
         <v>100000.0</v>
       </c>
       <c r="T64" s="1">
-        <v>100000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="U64" s="6">
-        <v>80000.0</v>
+        <v>32000.0</v>
       </c>
       <c r="V64" s="2"/>
       <c r="W64" s="1">
@@ -5425,7 +5476,7 @@
       </c>
       <c r="AE64"/>
       <c r="AF64">
-        <v>0.44</v>
+        <v>0.26</v>
       </c>
       <c r="AG64"/>
     </row>
@@ -5437,7 +5488,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="5">
@@ -5466,20 +5517,20 @@
       </c>
       <c r="O65" s="2"/>
       <c r="P65" s="6">
-        <v>100000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="Q65" s="2"/>
       <c r="R65" s="1">
-        <v>100000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="S65" s="1">
         <v>100000.0</v>
       </c>
       <c r="T65" s="1">
-        <v>100000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="U65" s="6">
-        <v>80000.0</v>
+        <v>28000.0</v>
       </c>
       <c r="V65" s="2"/>
       <c r="W65" s="1">
@@ -5504,7 +5555,7 @@
       </c>
       <c r="AE65"/>
       <c r="AF65">
-        <v>0.44</v>
+        <v>0.27</v>
       </c>
       <c r="AG65"/>
     </row>
@@ -5516,7 +5567,7 @@
         <v>76</v>
       </c>
       <c r="C66" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="5">
@@ -5545,20 +5596,20 @@
       </c>
       <c r="O66" s="2"/>
       <c r="P66" s="6">
-        <v>100000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="Q66" s="2"/>
       <c r="R66" s="1">
-        <v>100000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="S66" s="1">
         <v>100000.0</v>
       </c>
       <c r="T66" s="1">
-        <v>100000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="U66" s="6">
-        <v>80000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="V66" s="2"/>
       <c r="W66" s="1">
@@ -5583,7 +5634,7 @@
       </c>
       <c r="AE66"/>
       <c r="AF66">
-        <v>0.44</v>
+        <v>0.28</v>
       </c>
       <c r="AG66"/>
     </row>
@@ -5595,7 +5646,7 @@
         <v>77</v>
       </c>
       <c r="C67" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="5">
@@ -5624,20 +5675,20 @@
       </c>
       <c r="O67" s="2"/>
       <c r="P67" s="6">
-        <v>100000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="Q67" s="2"/>
       <c r="R67" s="1">
-        <v>100000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="S67" s="1">
         <v>100000.0</v>
       </c>
       <c r="T67" s="1">
-        <v>100000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="U67" s="6">
-        <v>80000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="V67" s="2"/>
       <c r="W67" s="1">
@@ -5662,7 +5713,7 @@
       </c>
       <c r="AE67"/>
       <c r="AF67">
-        <v>0.44</v>
+        <v>0.29</v>
       </c>
       <c r="AG67"/>
     </row>
@@ -5674,7 +5725,7 @@
         <v>78</v>
       </c>
       <c r="C68" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="5">
@@ -5703,20 +5754,20 @@
       </c>
       <c r="O68" s="2"/>
       <c r="P68" s="6">
-        <v>100000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="1">
-        <v>100000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="S68" s="1">
         <v>100000.0</v>
       </c>
       <c r="T68" s="1">
-        <v>100000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="U68" s="6">
-        <v>80000.0</v>
+        <v>16000.0</v>
       </c>
       <c r="V68" s="2"/>
       <c r="W68" s="1">
@@ -5741,7 +5792,7 @@
       </c>
       <c r="AE68"/>
       <c r="AF68">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
       <c r="AG68"/>
     </row>
@@ -5753,7 +5804,7 @@
         <v>79</v>
       </c>
       <c r="C69" s="4">
-        <v>33333.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="5">
@@ -5782,20 +5833,20 @@
       </c>
       <c r="O69" s="2"/>
       <c r="P69" s="6">
-        <v>66667.0</v>
+        <v>15000.0</v>
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="1">
-        <v>66667.0</v>
+        <v>15000.0</v>
       </c>
       <c r="S69" s="1">
         <v>100000.0</v>
       </c>
       <c r="T69" s="1">
-        <v>66667.0</v>
+        <v>15000.0</v>
       </c>
       <c r="U69" s="6">
-        <v>53333.6</v>
+        <v>12000.0</v>
       </c>
       <c r="V69" s="2"/>
       <c r="W69" s="1">
@@ -5820,7 +5871,7 @@
       </c>
       <c r="AE69"/>
       <c r="AF69">
-        <v>0.04</v>
+        <v>0.31</v>
       </c>
       <c r="AG69"/>
     </row>
@@ -5832,7 +5883,7 @@
         <v>80</v>
       </c>
       <c r="C70" s="4">
-        <v>33334.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="5">
@@ -5861,20 +5912,20 @@
       </c>
       <c r="O70" s="2"/>
       <c r="P70" s="6">
-        <v>33333.0</v>
+        <v>10000.0</v>
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="1">
-        <v>33333.0</v>
+        <v>10000.0</v>
       </c>
       <c r="S70" s="1">
         <v>100000.0</v>
       </c>
       <c r="T70" s="1">
-        <v>33333.0</v>
+        <v>10000.0</v>
       </c>
       <c r="U70" s="6">
-        <v>26666.4</v>
+        <v>8000.0</v>
       </c>
       <c r="V70" s="2"/>
       <c r="W70" s="1">
@@ -5899,7 +5950,7 @@
       </c>
       <c r="AE70"/>
       <c r="AF70">
-        <v>0.04</v>
+        <v>0.32</v>
       </c>
       <c r="AG70"/>
     </row>
@@ -5911,7 +5962,7 @@
         <v>81</v>
       </c>
       <c r="C71" s="4">
-        <v>33333.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="5">
@@ -5940,20 +5991,20 @@
       </c>
       <c r="O71" s="2"/>
       <c r="P71" s="6">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="Q71" s="2"/>
       <c r="R71" s="1">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="S71" s="1">
-        <v>0</v>
+        <v>100000.0</v>
       </c>
       <c r="T71" s="1">
-        <v>0</v>
+        <v>5000.0</v>
       </c>
       <c r="U71" s="6">
-        <v>0.0</v>
+        <v>4000.0</v>
       </c>
       <c r="V71" s="2"/>
       <c r="W71" s="1">
@@ -5978,7 +6029,7 @@
       </c>
       <c r="AE71"/>
       <c r="AF71">
-        <v>0.04</v>
+        <v>0.33</v>
       </c>
       <c r="AG71"/>
     </row>
@@ -5990,7 +6041,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="5">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D72" s="16"/>
       <c r="E72" s="5">
@@ -6056,7 +6107,9 @@
         <v>0.0</v>
       </c>
       <c r="AE72" s="15"/>
-      <c r="AF72" s="15"/>
+      <c r="AF72" s="15">
+        <v>0.35</v>
+      </c>
       <c r="AG72"/>
     </row>
     <row r="73" spans="1:33">
@@ -9821,7 +9874,7 @@
         <v>63</v>
       </c>
       <c r="C53" s="13">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="13">
@@ -9892,7 +9945,7 @@
         <v>64</v>
       </c>
       <c r="C54" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="5">
@@ -9962,7 +10015,7 @@
         <v>65</v>
       </c>
       <c r="C55" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="5">
@@ -10032,7 +10085,7 @@
         <v>66</v>
       </c>
       <c r="C56" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="5">
@@ -10102,7 +10155,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="13">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="13">
@@ -10173,7 +10226,7 @@
         <v>68</v>
       </c>
       <c r="C58" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="5">
@@ -10243,7 +10296,7 @@
         <v>69</v>
       </c>
       <c r="C59" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="5">
@@ -10313,7 +10366,7 @@
         <v>70</v>
       </c>
       <c r="C60" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="5">
@@ -10383,7 +10436,7 @@
         <v>71</v>
       </c>
       <c r="C61" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="5">
@@ -10453,7 +10506,7 @@
         <v>72</v>
       </c>
       <c r="C62" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="5">
@@ -10523,7 +10576,7 @@
         <v>73</v>
       </c>
       <c r="C63" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="5">
@@ -10593,7 +10646,7 @@
         <v>74</v>
       </c>
       <c r="C64" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="5">
@@ -10663,7 +10716,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="5">
@@ -10733,7 +10786,7 @@
         <v>76</v>
       </c>
       <c r="C66" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="5">
@@ -10803,7 +10856,7 @@
         <v>77</v>
       </c>
       <c r="C67" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="5">
@@ -10873,7 +10926,7 @@
         <v>78</v>
       </c>
       <c r="C68" s="4">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="5">
@@ -10943,7 +10996,7 @@
         <v>79</v>
       </c>
       <c r="C69" s="4">
-        <v>33333.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="5">
@@ -11013,7 +11066,7 @@
         <v>80</v>
       </c>
       <c r="C70" s="4">
-        <v>33334.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="5">
@@ -11083,7 +11136,7 @@
         <v>81</v>
       </c>
       <c r="C71" s="4">
-        <v>33333.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="5">
@@ -11153,7 +11206,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="5">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="D72" s="16"/>
       <c r="E72" s="5">
@@ -15081,26 +15134,26 @@
       <c r="N53" s="13"/>
       <c r="O53" s="14"/>
       <c r="P53" s="13">
-        <v>100000.0</v>
+        <v>95000.0</v>
       </c>
       <c r="Q53" s="14"/>
       <c r="R53" s="13">
-        <v>100000.0</v>
+        <v>95000.0</v>
       </c>
       <c r="S53" s="13">
         <v>100000.0</v>
       </c>
       <c r="T53" s="13">
-        <v>100000.0</v>
+        <v>95000.0</v>
       </c>
       <c r="U53" s="13">
-        <v>80000.0</v>
+        <v>76000.0</v>
       </c>
       <c r="V53" s="14">
         <v>0.8</v>
       </c>
       <c r="W53" s="13">
-        <v>800.0</v>
+        <v>760.0</v>
       </c>
       <c r="X53" s="14">
         <v>0.01</v>
@@ -15124,7 +15177,7 @@
       <c r="AE53" s="3"/>
       <c r="AF53" s="3"/>
       <c r="AG53" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:33">
@@ -15154,26 +15207,26 @@
       <c r="N54" s="1"/>
       <c r="O54" s="2"/>
       <c r="P54" s="6">
-        <v>100000.0</v>
+        <v>90000.0</v>
       </c>
       <c r="Q54" s="2"/>
       <c r="R54" s="1">
-        <v>100000.0</v>
+        <v>90000.0</v>
       </c>
       <c r="S54" s="1">
         <v>100000.0</v>
       </c>
       <c r="T54" s="1">
-        <v>100000.0</v>
+        <v>90000.0</v>
       </c>
       <c r="U54" s="6">
-        <v>80000.0</v>
+        <v>72000.0</v>
       </c>
       <c r="V54" s="2">
         <v>0.8</v>
       </c>
       <c r="W54" s="1">
-        <v>800.0</v>
+        <v>720.0</v>
       </c>
       <c r="X54" s="2">
         <v>0.01</v>
@@ -15196,7 +15249,7 @@
       </c>
       <c r="AE54"/>
       <c r="AG54" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:33">
@@ -15226,26 +15279,26 @@
       <c r="N55" s="1"/>
       <c r="O55" s="2"/>
       <c r="P55" s="6">
-        <v>100000.0</v>
+        <v>85000.0</v>
       </c>
       <c r="Q55" s="2"/>
       <c r="R55" s="1">
-        <v>100000.0</v>
+        <v>85000.0</v>
       </c>
       <c r="S55" s="1">
         <v>100000.0</v>
       </c>
       <c r="T55" s="1">
-        <v>100000.0</v>
+        <v>85000.0</v>
       </c>
       <c r="U55" s="6">
-        <v>80000.0</v>
+        <v>68000.0</v>
       </c>
       <c r="V55" s="2">
         <v>0.8</v>
       </c>
       <c r="W55" s="1">
-        <v>800.0</v>
+        <v>680.0</v>
       </c>
       <c r="X55" s="2">
         <v>0.01</v>
@@ -15268,7 +15321,7 @@
       </c>
       <c r="AE55"/>
       <c r="AG55" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:33">
@@ -15298,26 +15351,26 @@
       <c r="N56" s="1"/>
       <c r="O56" s="2"/>
       <c r="P56" s="6">
-        <v>100000.0</v>
+        <v>80000.0</v>
       </c>
       <c r="Q56" s="2"/>
       <c r="R56" s="1">
-        <v>100000.0</v>
+        <v>80000.0</v>
       </c>
       <c r="S56" s="1">
         <v>100000.0</v>
       </c>
       <c r="T56" s="1">
-        <v>100000.0</v>
+        <v>80000.0</v>
       </c>
       <c r="U56" s="6">
-        <v>80000.0</v>
+        <v>64000.0</v>
       </c>
       <c r="V56" s="2">
         <v>0.8</v>
       </c>
       <c r="W56" s="1">
-        <v>800.0</v>
+        <v>640.0</v>
       </c>
       <c r="X56" s="2">
         <v>0.01</v>
@@ -15340,7 +15393,7 @@
       </c>
       <c r="AE56"/>
       <c r="AG56" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:33">
@@ -15370,26 +15423,26 @@
       <c r="N57" s="13"/>
       <c r="O57" s="14"/>
       <c r="P57" s="13">
-        <v>100000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="Q57" s="14"/>
       <c r="R57" s="13">
-        <v>100000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="S57" s="13">
         <v>100000.0</v>
       </c>
       <c r="T57" s="13">
-        <v>100000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="U57" s="13">
-        <v>80000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="V57" s="14">
         <v>0.8</v>
       </c>
       <c r="W57" s="13">
-        <v>800.0</v>
+        <v>600.0</v>
       </c>
       <c r="X57" s="14">
         <v>0.01</v>
@@ -15413,7 +15466,7 @@
       <c r="AE57" s="3"/>
       <c r="AF57" s="3"/>
       <c r="AG57" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:33">
@@ -15443,26 +15496,26 @@
       <c r="N58" s="1"/>
       <c r="O58" s="2"/>
       <c r="P58" s="6">
-        <v>100000.0</v>
+        <v>70000.0</v>
       </c>
       <c r="Q58" s="2"/>
       <c r="R58" s="1">
-        <v>100000.0</v>
+        <v>70000.0</v>
       </c>
       <c r="S58" s="1">
         <v>100000.0</v>
       </c>
       <c r="T58" s="1">
-        <v>100000.0</v>
+        <v>70000.0</v>
       </c>
       <c r="U58" s="6">
-        <v>80000.0</v>
+        <v>56000.0</v>
       </c>
       <c r="V58" s="2">
         <v>0.8</v>
       </c>
       <c r="W58" s="1">
-        <v>800.0</v>
+        <v>560.0</v>
       </c>
       <c r="X58" s="2">
         <v>0.01</v>
@@ -15485,7 +15538,7 @@
       </c>
       <c r="AE58"/>
       <c r="AG58" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:33">
@@ -15515,26 +15568,26 @@
       <c r="N59" s="1"/>
       <c r="O59" s="2"/>
       <c r="P59" s="6">
-        <v>100000.0</v>
+        <v>65000.0</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="1">
-        <v>100000.0</v>
+        <v>65000.0</v>
       </c>
       <c r="S59" s="1">
         <v>100000.0</v>
       </c>
       <c r="T59" s="1">
-        <v>100000.0</v>
+        <v>65000.0</v>
       </c>
       <c r="U59" s="6">
-        <v>80000.0</v>
+        <v>52000.0</v>
       </c>
       <c r="V59" s="2">
         <v>0.8</v>
       </c>
       <c r="W59" s="1">
-        <v>800.0</v>
+        <v>520.0</v>
       </c>
       <c r="X59" s="2">
         <v>0.01</v>
@@ -15557,7 +15610,7 @@
       </c>
       <c r="AE59"/>
       <c r="AG59" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:33">
@@ -15587,26 +15640,26 @@
       <c r="N60" s="1"/>
       <c r="O60" s="2"/>
       <c r="P60" s="6">
-        <v>100000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="1">
-        <v>100000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="S60" s="1">
         <v>100000.0</v>
       </c>
       <c r="T60" s="1">
-        <v>100000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="U60" s="6">
-        <v>80000.0</v>
+        <v>48000.0</v>
       </c>
       <c r="V60" s="2">
         <v>0.8</v>
       </c>
       <c r="W60" s="1">
-        <v>800.0</v>
+        <v>480.0</v>
       </c>
       <c r="X60" s="2">
         <v>0.01</v>
@@ -15629,7 +15682,7 @@
       </c>
       <c r="AE60"/>
       <c r="AG60" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:33">
@@ -15659,26 +15712,26 @@
       <c r="N61" s="1"/>
       <c r="O61" s="2"/>
       <c r="P61" s="6">
-        <v>100000.0</v>
+        <v>55000.0</v>
       </c>
       <c r="Q61" s="2"/>
       <c r="R61" s="1">
-        <v>100000.0</v>
+        <v>55000.0</v>
       </c>
       <c r="S61" s="1">
         <v>100000.0</v>
       </c>
       <c r="T61" s="1">
-        <v>100000.0</v>
+        <v>55000.0</v>
       </c>
       <c r="U61" s="6">
-        <v>80000.0</v>
+        <v>44000.0</v>
       </c>
       <c r="V61" s="2">
         <v>0.8</v>
       </c>
       <c r="W61" s="1">
-        <v>800.0</v>
+        <v>440.0</v>
       </c>
       <c r="X61" s="2">
         <v>0.01</v>
@@ -15701,7 +15754,7 @@
       </c>
       <c r="AE61"/>
       <c r="AG61" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:33">
@@ -15731,26 +15784,26 @@
       <c r="N62" s="1"/>
       <c r="O62" s="2"/>
       <c r="P62" s="6">
-        <v>100000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="1">
-        <v>100000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="S62" s="1">
         <v>100000.0</v>
       </c>
       <c r="T62" s="1">
-        <v>100000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="U62" s="6">
-        <v>80000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="V62" s="2">
         <v>0.8</v>
       </c>
       <c r="W62" s="1">
-        <v>800.0</v>
+        <v>400.0</v>
       </c>
       <c r="X62" s="2">
         <v>0.01</v>
@@ -15773,7 +15826,7 @@
       </c>
       <c r="AE62"/>
       <c r="AG62" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:33">
@@ -15803,26 +15856,26 @@
       <c r="N63" s="1"/>
       <c r="O63" s="2"/>
       <c r="P63" s="6">
-        <v>100000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="Q63" s="2"/>
       <c r="R63" s="1">
-        <v>100000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="S63" s="1">
         <v>100000.0</v>
       </c>
       <c r="T63" s="1">
-        <v>100000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="U63" s="6">
-        <v>80000.0</v>
+        <v>36000.0</v>
       </c>
       <c r="V63" s="2">
         <v>0.8</v>
       </c>
       <c r="W63" s="1">
-        <v>800.0</v>
+        <v>360.0</v>
       </c>
       <c r="X63" s="2">
         <v>0.01</v>
@@ -15845,7 +15898,7 @@
       </c>
       <c r="AE63"/>
       <c r="AG63" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:33">
@@ -15875,26 +15928,26 @@
       <c r="N64" s="1"/>
       <c r="O64" s="2"/>
       <c r="P64" s="6">
-        <v>100000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="Q64" s="2"/>
       <c r="R64" s="1">
-        <v>100000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="S64" s="1">
         <v>100000.0</v>
       </c>
       <c r="T64" s="1">
-        <v>100000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="U64" s="6">
-        <v>80000.0</v>
+        <v>32000.0</v>
       </c>
       <c r="V64" s="2">
         <v>0.8</v>
       </c>
       <c r="W64" s="1">
-        <v>800.0</v>
+        <v>320.0</v>
       </c>
       <c r="X64" s="2">
         <v>0.01</v>
@@ -15917,7 +15970,7 @@
       </c>
       <c r="AE64"/>
       <c r="AG64" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:33">
@@ -15947,26 +16000,26 @@
       <c r="N65" s="1"/>
       <c r="O65" s="2"/>
       <c r="P65" s="6">
-        <v>100000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="Q65" s="2"/>
       <c r="R65" s="1">
-        <v>100000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="S65" s="1">
         <v>100000.0</v>
       </c>
       <c r="T65" s="1">
-        <v>100000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="U65" s="6">
-        <v>80000.0</v>
+        <v>28000.0</v>
       </c>
       <c r="V65" s="2">
         <v>0.8</v>
       </c>
       <c r="W65" s="1">
-        <v>800.0</v>
+        <v>280.0</v>
       </c>
       <c r="X65" s="2">
         <v>0.01</v>
@@ -15989,7 +16042,7 @@
       </c>
       <c r="AE65"/>
       <c r="AG65" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:33">
@@ -16019,26 +16072,26 @@
       <c r="N66" s="1"/>
       <c r="O66" s="2"/>
       <c r="P66" s="6">
-        <v>100000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="Q66" s="2"/>
       <c r="R66" s="1">
-        <v>100000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="S66" s="1">
         <v>100000.0</v>
       </c>
       <c r="T66" s="1">
-        <v>100000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="U66" s="6">
-        <v>80000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="V66" s="2">
         <v>0.8</v>
       </c>
       <c r="W66" s="1">
-        <v>800.0</v>
+        <v>240.0</v>
       </c>
       <c r="X66" s="2">
         <v>0.01</v>
@@ -16061,7 +16114,7 @@
       </c>
       <c r="AE66"/>
       <c r="AG66" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:33">
@@ -16091,26 +16144,26 @@
       <c r="N67" s="1"/>
       <c r="O67" s="2"/>
       <c r="P67" s="6">
-        <v>100000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="Q67" s="2"/>
       <c r="R67" s="1">
-        <v>100000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="S67" s="1">
         <v>100000.0</v>
       </c>
       <c r="T67" s="1">
-        <v>100000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="U67" s="6">
-        <v>80000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="V67" s="2">
         <v>0.8</v>
       </c>
       <c r="W67" s="1">
-        <v>800.0</v>
+        <v>200.0</v>
       </c>
       <c r="X67" s="2">
         <v>0.01</v>
@@ -16133,7 +16186,7 @@
       </c>
       <c r="AE67"/>
       <c r="AG67" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:33">
@@ -16163,26 +16216,26 @@
       <c r="N68" s="1"/>
       <c r="O68" s="2"/>
       <c r="P68" s="6">
-        <v>100000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="1">
-        <v>100000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="S68" s="1">
         <v>100000.0</v>
       </c>
       <c r="T68" s="1">
-        <v>100000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="U68" s="6">
-        <v>80000.0</v>
+        <v>16000.0</v>
       </c>
       <c r="V68" s="2">
         <v>0.8</v>
       </c>
       <c r="W68" s="1">
-        <v>800.0</v>
+        <v>160.0</v>
       </c>
       <c r="X68" s="2">
         <v>0.01</v>
@@ -16205,7 +16258,7 @@
       </c>
       <c r="AE68"/>
       <c r="AG68" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:33">
@@ -16235,26 +16288,26 @@
       <c r="N69" s="1"/>
       <c r="O69" s="2"/>
       <c r="P69" s="6">
-        <v>66667.0</v>
+        <v>15000.0</v>
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="1">
-        <v>66667.0</v>
+        <v>15000.0</v>
       </c>
       <c r="S69" s="1">
         <v>100000.0</v>
       </c>
       <c r="T69" s="1">
-        <v>66667.0</v>
+        <v>15000.0</v>
       </c>
       <c r="U69" s="6">
-        <v>53333.6</v>
+        <v>12000.0</v>
       </c>
       <c r="V69" s="2">
         <v>0.8</v>
       </c>
       <c r="W69" s="1">
-        <v>533.336</v>
+        <v>120.0</v>
       </c>
       <c r="X69" s="2">
         <v>0.01</v>
@@ -16277,7 +16330,7 @@
       </c>
       <c r="AE69"/>
       <c r="AG69" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:33">
@@ -16307,26 +16360,26 @@
       <c r="N70" s="1"/>
       <c r="O70" s="2"/>
       <c r="P70" s="6">
-        <v>33333.0</v>
+        <v>10000.0</v>
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="1">
-        <v>33333.0</v>
+        <v>10000.0</v>
       </c>
       <c r="S70" s="1">
         <v>100000.0</v>
       </c>
       <c r="T70" s="1">
-        <v>33333.0</v>
+        <v>10000.0</v>
       </c>
       <c r="U70" s="6">
-        <v>26666.4</v>
+        <v>8000.0</v>
       </c>
       <c r="V70" s="2">
         <v>0.8</v>
       </c>
       <c r="W70" s="1">
-        <v>266.664</v>
+        <v>80.0</v>
       </c>
       <c r="X70" s="2">
         <v>0.01</v>
@@ -16349,7 +16402,7 @@
       </c>
       <c r="AE70"/>
       <c r="AG70" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:33">
@@ -16379,26 +16432,30 @@
       <c r="N71" s="1"/>
       <c r="O71" s="2"/>
       <c r="P71" s="6">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="Q71" s="2"/>
       <c r="R71" s="1">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="S71" s="1">
-        <v>0</v>
+        <v>100000.0</v>
       </c>
       <c r="T71" s="1">
-        <v>0</v>
+        <v>5000.0</v>
       </c>
       <c r="U71" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="V71" s="2"/>
+        <v>4000.0</v>
+      </c>
+      <c r="V71" s="2">
+        <v>0.8</v>
+      </c>
       <c r="W71" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="X71" s="2"/>
+        <v>40.0</v>
+      </c>
+      <c r="X71" s="2">
+        <v>0.01</v>
+      </c>
       <c r="Y71" s="1">
         <v>0</v>
       </c>
@@ -16417,7 +16474,7 @@
       </c>
       <c r="AE71"/>
       <c r="AG71" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:33">
@@ -16486,7 +16543,7 @@
       <c r="AE72" s="15"/>
       <c r="AF72" s="15"/>
       <c r="AG72" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:33">
@@ -16763,7 +16820,7 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -17472,6 +17529,12 @@
     <row r="71" spans="1:3">
       <c r="A71">
         <v>2086</v>
+      </c>
+      <c r="B71">
+        <v>100.0</v>
+      </c>
+      <c r="C71">
+        <v>100.0</v>
       </c>
     </row>
     <row r="72" spans="1:3">

</xml_diff>